<commit_message>
Terminando a Formatação do Texto do Backlog
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -93,16 +93,9 @@
     <t>Sprint 2 - Camada Login e Cadastro</t>
   </si>
   <si>
-    <t>Estipular o tema e criar o Termo de Abertura do Projeto.</t>
-  </si>
-  <si>
     <t>Criar Product Backlog</t>
   </si>
   <si>
-    <t xml:space="preserve">Configurar e Organizar o GitHub e Ferramenta de Gestão do Projeto.
-</t>
-  </si>
-  <si>
     <t>02211038</t>
   </si>
   <si>
@@ -122,9 +115,6 @@
   </si>
   <si>
     <t>Desenvolver Principais Subjects do Login: "input_user_login" e "model_login"</t>
-  </si>
-  <si>
-    <t>Criar o banco de dados em seu modelo lógico e físico.</t>
   </si>
   <si>
     <t>Finalizar toda Documentação inicial e a Camada do Jogo</t>
@@ -191,13 +181,23 @@
     <t>Fazer Bateria de Testes Unitarios nas Camadas de Cadastro e Login de Usuarios</t>
   </si>
   <si>
-    <t>Fazer Bateria de Testes de Integração entre as 3 Camadas: Jogo, Login e Cadastro.</t>
-  </si>
-  <si>
     <t>Fazer Bateria de Testes Unitarios na Camada Jogo</t>
   </si>
   <si>
     <t>Concluir Projeto - "Space-Invaders-Bullet-Hell"</t>
+  </si>
+  <si>
+    <t>Estipular o tema e criar o Termo de Abertura do Projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configurar e Organizar o GitHub e Ferramenta de Gestão do Projeto
+</t>
+  </si>
+  <si>
+    <t>Criar o banco de dados em seu modelo lógico e físico</t>
+  </si>
+  <si>
+    <t>Fazer Bateria de Testes de Integração entre as 3 Camadas: Jogo, Login e Cadastro</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,7 +718,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -769,7 +769,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1">
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>6</v>
@@ -793,7 +793,7 @@
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>18</v>
@@ -807,7 +807,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>6</v>
@@ -828,7 +828,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>6</v>
@@ -849,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>6</v>
@@ -870,7 +870,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>6</v>
@@ -891,7 +891,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>21</v>
@@ -912,7 +912,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
@@ -933,7 +933,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>6</v>
@@ -954,14 +954,14 @@
         <v>14</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F12" s="18">
         <v>44325</v>
@@ -1004,7 +1004,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>6</v>
@@ -1025,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>6</v>
@@ -1046,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>6</v>
@@ -1067,7 +1067,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>21</v>
@@ -1088,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>6</v>
@@ -1109,7 +1109,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>21</v>
@@ -1130,7 +1130,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>21</v>
@@ -1151,7 +1151,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>6</v>
@@ -1172,14 +1172,14 @@
         <v>14</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F24" s="18">
         <v>44330</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="B26" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
@@ -1222,7 +1222,7 @@
         <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>6</v>
@@ -1243,7 +1243,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>6</v>
@@ -1264,7 +1264,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>6</v>
@@ -1285,7 +1285,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>21</v>
@@ -1306,7 +1306,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>21</v>
@@ -1327,7 +1327,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>21</v>
@@ -1348,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>6</v>
@@ -1369,7 +1369,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>6</v>
@@ -1390,7 +1390,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>6</v>
@@ -1408,10 +1408,10 @@
     </row>
     <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>6</v>
@@ -1429,17 +1429,17 @@
     </row>
     <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F38" s="18">
         <v>44336</v>

</xml_diff>

<commit_message>
Fazendo Pequenos Ajustes no Backlog
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -111,12 +111,6 @@
     <t>MAX</t>
   </si>
   <si>
-    <t>Desenvolver Principais Subjects do Cadastro: "input_user_register" e "model_register"</t>
-  </si>
-  <si>
-    <t>Desenvolver Principais Subjects do Login: "input_user_login" e "model_login"</t>
-  </si>
-  <si>
     <t>Finalizar toda Documentação inicial e a Camada do Jogo</t>
   </si>
   <si>
@@ -130,10 +124,6 @@
   </si>
   <si>
     <t xml:space="preserve">Desenvolver um Fluxograma em linha de prioridade de "Atendimento do Suporte"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver Principais Subjects do Jogo: "input_user_keyboard", "model_game"
-e "render_screen" </t>
   </si>
   <si>
     <t>Relacionar os arquivos do diretorio "game_layer" com o controller e depois com o server</t>
@@ -198,6 +188,16 @@
   </si>
   <si>
     <t>Fazer Bateria de Testes de Integração entre as 3 Camadas: Jogo, Login e Cadastro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver Principais Models e Inputs da camada Jogo: "input_user_keyboard", "model_game"
+e "render_screen" </t>
+  </si>
+  <si>
+    <t>Desenvolver Principais Models e Inputs da camada Login: "input_user_login" e "model_login"</t>
+  </si>
+  <si>
+    <t>Desenvolver Principais  Models e Inputs da camada Cadastro: "input_user_register" e "model_register"</t>
   </si>
 </sst>
 </file>
@@ -257,7 +257,7 @@
       <name val="Biome"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +300,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -328,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -386,6 +392,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -717,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -769,7 +787,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1">
@@ -777,7 +795,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>6</v>
@@ -806,19 +824,19 @@
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="B5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="22">
         <v>3</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="22">
         <v>2</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="23">
         <v>44314</v>
       </c>
       <c r="G5" s="11"/>
@@ -827,19 +845,19 @@
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="C6" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="22">
         <v>13</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="22">
         <v>3</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="23">
         <v>44315</v>
       </c>
       <c r="G6" s="11"/>
@@ -848,19 +866,19 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="22">
         <v>8</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="22">
         <v>4</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="23">
         <v>44316</v>
       </c>
       <c r="G7" s="11"/>
@@ -870,7 +888,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>6</v>
@@ -891,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>21</v>
@@ -912,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
@@ -954,7 +972,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="17" t="s">
@@ -1025,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>6</v>
@@ -1046,7 +1064,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>6</v>
@@ -1067,7 +1085,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>21</v>
@@ -1088,7 +1106,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>6</v>
@@ -1109,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>21</v>
@@ -1130,7 +1148,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>21</v>
@@ -1151,7 +1169,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>6</v>
@@ -1172,7 +1190,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="17" t="s">
@@ -1191,7 +1209,7 @@
     </row>
     <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="B26" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
@@ -1222,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>6</v>
@@ -1243,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>6</v>
@@ -1264,7 +1282,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>6</v>
@@ -1285,7 +1303,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>21</v>
@@ -1306,7 +1324,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>21</v>
@@ -1327,7 +1345,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>21</v>
@@ -1348,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>6</v>
@@ -1369,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>6</v>
@@ -1390,7 +1408,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>6</v>
@@ -1408,10 +1426,10 @@
     </row>
     <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>6</v>
@@ -1429,10 +1447,10 @@
     </row>
     <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="17" t="s">

</xml_diff>

<commit_message>
Fazendo Pequenos Acertos no Backlog
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -102,12 +102,6 @@
     <t>Criar HLD/LLD do Projeto</t>
   </si>
   <si>
-    <t>Desenvolver o Front-End das Paginas: "index",  "login_page" e "register_page"</t>
-  </si>
-  <si>
-    <t>Desenvolver o Basico do Front-End da Pagina: "game_screen"</t>
-  </si>
-  <si>
     <t>MAX</t>
   </si>
   <si>
@@ -126,12 +120,6 @@
     <t xml:space="preserve">Desenvolver um Fluxograma em linha de prioridade de "Atendimento do Suporte"  </t>
   </si>
   <si>
-    <t>Relacionar os arquivos do diretorio "game_layer" com o controller e depois com o server</t>
-  </si>
-  <si>
-    <t>Relacionar os arquivos dos diretorios "user_register_layer" e "user_login_layer" com o controller e depois com o server</t>
-  </si>
-  <si>
     <t xml:space="preserve">Criar o Arquivo PPT da Apresentação. Lembrando dos Temas pedidos na Apresentação pela Materia Socioemocional </t>
   </si>
   <si>
@@ -160,9 +148,6 @@
   </si>
   <si>
     <t>Criar uma POC utilizando Métricas Aplicadas aos Dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fazer o Mapeamento das Tabelas (entidades) em classes JavaScript </t>
   </si>
   <si>
     <t>Apresentar o Projeto para a Banca</t>
@@ -184,20 +169,35 @@
 </t>
   </si>
   <si>
-    <t>Criar o banco de dados em seu modelo lógico e físico</t>
-  </si>
-  <si>
     <t>Fazer Bateria de Testes de Integração entre as 3 Camadas: Jogo, Login e Cadastro</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver Principais Models e Inputs da camada Jogo: "input_user_keyboard", "model_game"
+    <t>Relacionar os arquivos do diretorio "game_layer" com o controller e depois com o server.js</t>
+  </si>
+  <si>
+    <t>Desenvolver uma Camada de View Basica para a Pagina: "game_screen"</t>
+  </si>
+  <si>
+    <t>Desenvolver a Camada de View das Paginas: "index",  "login_page" e "register_page"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver as Regras de Negocio da Camada do Jogo: "input_user_keyboard", "model_game"
 e "render_screen" </t>
   </si>
   <si>
-    <t>Desenvolver Principais Models e Inputs da camada Login: "input_user_login" e "model_login"</t>
-  </si>
-  <si>
-    <t>Desenvolver Principais  Models e Inputs da camada Cadastro: "input_user_register" e "model_register"</t>
+    <t>Desenvolver Principais  as Regras de Negocio da camada Cadastro: "input_user_register" e "model_register"</t>
+  </si>
+  <si>
+    <t>Desenvolver as Regras de Negocio da camada Login: "input_user_login" e "model_login"</t>
+  </si>
+  <si>
+    <t>Relacionar os arquivos dos diretorios "user_register_layer" e "user_login_layer" com o controller e depois com o server.js</t>
+  </si>
+  <si>
+    <t>Criar o banco de dados em seu modelo lógico, Dicionario de Dados e Banco Físico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer o Model com o Mapeamento das Tabelas (entidades) em classes JavaScript </t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -787,26 +787,26 @@
         <v>19</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="B4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="22">
         <v>8</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="22">
         <v>1</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="23">
         <v>44313</v>
       </c>
       <c r="G4" s="11"/>
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>6</v>
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
@@ -888,7 +888,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>6</v>
@@ -909,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>21</v>
@@ -930,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
@@ -972,14 +972,14 @@
         <v>14</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="18">
         <v>44325</v>
@@ -1022,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>6</v>
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>6</v>
@@ -1064,7 +1064,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>6</v>
@@ -1085,7 +1085,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>21</v>
@@ -1106,7 +1106,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>6</v>
@@ -1127,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>21</v>
@@ -1148,7 +1148,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>21</v>
@@ -1169,7 +1169,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>6</v>
@@ -1190,14 +1190,14 @@
         <v>14</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F24" s="18">
         <v>44330</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="B26" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
@@ -1240,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>6</v>
@@ -1261,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>6</v>
@@ -1282,7 +1282,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>6</v>
@@ -1303,7 +1303,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>21</v>
@@ -1324,7 +1324,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>21</v>
@@ -1345,7 +1345,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>21</v>
@@ -1366,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>6</v>
@@ -1387,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>6</v>
@@ -1408,7 +1408,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>6</v>
@@ -1426,10 +1426,10 @@
     </row>
     <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>6</v>
@@ -1447,17 +1447,17 @@
     </row>
     <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F38" s="18">
         <v>44336</v>

</xml_diff>

<commit_message>
Atualizando Avanço do Backlog
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -725,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -736,7 +736,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -908,19 +908,19 @@
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="22">
         <v>13</v>
       </c>
-      <c r="E9" s="11">
-        <v>6</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="22">
+        <v>6</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="11"/>

</xml_diff>

<commit_message>
Atualizando Backlog e Pequenas alterações no sql.script
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -337,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -416,6 +416,9 @@
     </xf>
     <xf numFmtId="16" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -747,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -1054,19 +1057,19 @@
       <c r="A17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="11">
+      <c r="C17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="22">
         <v>13</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="22">
         <v>1</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="23">
         <v>44326</v>
       </c>
       <c r="G17" s="11"/>
@@ -1117,19 +1120,19 @@
       <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="22">
         <v>13</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="22">
         <v>4</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="23" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="11"/>

</xml_diff>

<commit_message>
Atualizando e Fazendo Pequenas Alterações no Backlog
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -120,9 +120,6 @@
     <t xml:space="preserve">Desenvolver um Fluxograma em linha de prioridade de "Atendimento do Suporte"  </t>
   </si>
   <si>
-    <t xml:space="preserve">Criar o Arquivo PPT da Apresentação. Lembrando dos Temas pedidos na Apresentação pela Materia Socioemocional </t>
-  </si>
-  <si>
     <t>RF10</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
   </si>
   <si>
     <t>Criar uma POC utilizando Métricas Aplicadas aos Dados</t>
-  </si>
-  <si>
-    <t>Apresentar o Projeto para a Banca</t>
   </si>
   <si>
     <t>Fazer Bateria de Testes Unitarios nas Camadas de Cadastro e Login de Usuarios</t>
@@ -740,7 +734,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -748,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J39"/>
+  <dimension ref="A2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -802,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1">
@@ -810,7 +804,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>6</v>
@@ -840,7 +834,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>6</v>
@@ -882,7 +876,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
@@ -903,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>6</v>
@@ -924,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>21</v>
@@ -944,19 +938,19 @@
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="22">
         <v>13</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="22">
         <v>7</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="22" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="11"/>
@@ -966,7 +960,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>21</v>
@@ -1005,7 +999,7 @@
     </row>
     <row r="13" spans="1:10" ht="39.950000000000003" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>28</v>
@@ -1058,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>6</v>
@@ -1078,19 +1072,19 @@
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="11">
+      <c r="B18" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="22">
         <v>8</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="22">
         <v>2</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="23">
         <v>44326</v>
       </c>
       <c r="G18" s="11"/>
@@ -1099,19 +1093,19 @@
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="11">
+      <c r="B19" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="22">
         <v>8</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="22">
         <v>3</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="23">
         <v>44327</v>
       </c>
       <c r="G19" s="11"/>
@@ -1121,7 +1115,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>21</v>
@@ -1142,7 +1136,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>6</v>
@@ -1163,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>21</v>
@@ -1184,7 +1178,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>21</v>
@@ -1205,7 +1199,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>6</v>
@@ -1226,7 +1220,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="17" t="s">
@@ -1276,7 +1270,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>6</v>
@@ -1339,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>21</v>
@@ -1360,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>21</v>
@@ -1381,7 +1375,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>21</v>
@@ -1402,7 +1396,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>6</v>
@@ -1441,66 +1435,24 @@
     </row>
     <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="11">
-        <v>8</v>
-      </c>
-      <c r="E37" s="11">
-        <v>9</v>
-      </c>
-      <c r="F37" s="14">
-        <v>44304</v>
-      </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A38" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="11">
-        <v>13</v>
-      </c>
-      <c r="E38" s="11">
-        <v>10</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A39" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E37" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F37" s="18">
         <v>44336</v>
       </c>
-      <c r="G39" s="17">
-        <f>SUM(D29:D38)</f>
-        <v>131</v>
+      <c r="G37" s="17">
+        <f>SUM(D29:D36)</f>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organizando Documentação do Projeto e do Banco de Dados, além de tirar dependencias que não estão sendo utilizadas
</commit_message>
<xml_diff>
--- a/doc/project_docs/2.Product-Backlog.xlsx
+++ b/doc/project_docs/2.Product-Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -120,9 +120,6 @@
     <t xml:space="preserve">Desenvolver um Fluxograma em linha de prioridade de "Atendimento do Suporte"  </t>
   </si>
   <si>
-    <t>RF10</t>
-  </si>
-  <si>
     <t>Prazo Final:</t>
   </si>
   <si>
@@ -132,25 +129,7 @@
     <t xml:space="preserve">Finalizar toda Parte de Cadastro, Login, Banco de Dados e os Documentos Intermediarios </t>
   </si>
   <si>
-    <t>RF11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fazer Bateria de Testes Unitarios </t>
-  </si>
-  <si>
-    <t>Fazer Bateria de Testes de Integração entre: Aplicação, API e Banco de Dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fazer Testes "END-TO-END" </t>
-  </si>
-  <si>
     <t>Criar uma POC utilizando Métricas Aplicadas aos Dados</t>
-  </si>
-  <si>
-    <t>Fazer Bateria de Testes Unitarios nas Camadas de Cadastro e Login de Usuarios</t>
-  </si>
-  <si>
-    <t>Fazer Bateria de Testes Unitarios na Camada Jogo</t>
   </si>
   <si>
     <t>Concluir Projeto - "Space-Invaders-Bullet-Hell"</t>
@@ -163,38 +142,31 @@
 </t>
   </si>
   <si>
-    <t>Fazer Bateria de Testes de Integração entre as 3 Camadas: Jogo, Login e Cadastro</t>
-  </si>
-  <si>
     <t>Relacionar os arquivos do diretorio "game_layer" com o controller e depois com o server.js</t>
   </si>
   <si>
-    <t>Desenvolver uma Camada de View Basica para a Pagina: "game_screen"</t>
-  </si>
-  <si>
-    <t>Desenvolver a Camada de View das Paginas: "index",  "login_page" e "register_page"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver as Regras de Negocio da Camada do Jogo: "input_user_keyboard", "model_game"
-e "render_screen" </t>
-  </si>
-  <si>
-    <t>Desenvolver Principais  as Regras de Negocio da camada Cadastro: "input_user_register" e "model_register"</t>
-  </si>
-  <si>
-    <t>Desenvolver as Regras de Negocio da camada Login: "input_user_login" e "model_login"</t>
-  </si>
-  <si>
     <t>Relacionar os arquivos dos diretorios "user_register_layer" e "user_login_layer" com o controller e depois com o server.js</t>
   </si>
   <si>
-    <t>Criar o banco de dados em seu modelo lógico, Dicionario de Dados e Banco Físico</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fazer o Model com o Mapeamento das Tabelas (entidades) em classes JavaScript </t>
   </si>
   <si>
     <t>Aprimorar os Scripts com Regras de Negocio do Jogo para Javascript Modules</t>
+  </si>
+  <si>
+    <t>Desenvolver uma Camada de View Basica para a Pagina: "client_game"</t>
+  </si>
+  <si>
+    <t>Desenvolver as Regras de Negocio da Camada do Jogo: "brules_game",  "input_user_keyboard" e "render_screen"</t>
+  </si>
+  <si>
+    <t>Desenvolver a Camada de View das Paginas: "index" e "register_page"</t>
+  </si>
+  <si>
+    <t>Desenvolver as Regras de Negocio da camada Login: "brules_login".</t>
+  </si>
+  <si>
+    <t>Criar o banco de dados em seu modelo lógico, Banco Físico e Dicionario de Dados</t>
   </si>
 </sst>
 </file>
@@ -254,7 +226,7 @@
       <name val="Biome"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,12 +254,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -354,7 +320,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,9 +333,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -390,16 +353,16 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -411,7 +374,7 @@
     <xf numFmtId="16" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -742,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J37"/>
+  <dimension ref="A2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -795,27 +758,27 @@
       <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>34</v>
+      <c r="J3" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="22">
+      <c r="B4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="21">
         <v>8</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <v>1</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>44313</v>
       </c>
       <c r="G4" s="11"/>
@@ -825,7 +788,7 @@
       <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>44336</v>
       </c>
     </row>
@@ -833,19 +796,19 @@
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="22">
+      <c r="B5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="21">
         <v>3</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>2</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>44314</v>
       </c>
       <c r="G5" s="11"/>
@@ -854,19 +817,19 @@
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="22">
+      <c r="C6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="21">
         <v>13</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="21">
         <v>3</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <v>44315</v>
       </c>
       <c r="G6" s="11"/>
@@ -875,19 +838,19 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="22">
+      <c r="B7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="21">
         <v>8</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>4</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <v>44316</v>
       </c>
       <c r="G7" s="11"/>
@@ -896,19 +859,19 @@
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="22">
+      <c r="B8" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="21">
         <v>21</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>5</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>44323</v>
       </c>
       <c r="G8" s="11"/>
@@ -917,19 +880,19 @@
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>13</v>
       </c>
-      <c r="E9" s="22">
-        <v>6</v>
-      </c>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="21">
+        <v>6</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="11"/>
@@ -938,19 +901,19 @@
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>13</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <v>7</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="11"/>
@@ -959,20 +922,20 @@
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="11">
+      <c r="B11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="24">
+        <v>5</v>
+      </c>
+      <c r="E11" s="24">
         <v>8</v>
       </c>
-      <c r="E11" s="11">
-        <v>7</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>15</v>
+      <c r="F11" s="25">
+        <v>44324</v>
       </c>
       <c r="G11" s="11"/>
     </row>
@@ -980,479 +943,332 @@
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="25">
+      <c r="B12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="17">
+        <v>44325</v>
+      </c>
+      <c r="G12" s="16">
+        <f>SUM(D4:D11)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="39.950000000000003" customHeight="1">
+      <c r="B14" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="39.950000000000003" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="39.950000000000003" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="25">
-        <v>8</v>
-      </c>
-      <c r="F12" s="26">
-        <v>44324</v>
-      </c>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="39.950000000000003" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="18">
-        <v>44325</v>
-      </c>
-      <c r="G13" s="17">
-        <f>SUM(D4:D12)</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="39.950000000000003" customHeight="1">
-      <c r="B15" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="39.950000000000003" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="21">
+        <v>13</v>
+      </c>
+      <c r="E16" s="21">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="F16" s="22">
+        <v>44326</v>
+      </c>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="22">
-        <v>13</v>
-      </c>
-      <c r="E17" s="22">
-        <v>1</v>
-      </c>
-      <c r="F17" s="23">
-        <v>44326</v>
+        <v>7</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="21">
+        <v>8</v>
+      </c>
+      <c r="E17" s="21">
+        <v>3</v>
+      </c>
+      <c r="F17" s="22">
+        <v>44327</v>
       </c>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="22">
         <v>8</v>
       </c>
-      <c r="E18" s="22">
-        <v>2</v>
-      </c>
-      <c r="F18" s="23">
-        <v>44326</v>
+      <c r="B18" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="21">
+        <v>13</v>
+      </c>
+      <c r="E18" s="21">
+        <v>4</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="22">
-        <v>8</v>
-      </c>
-      <c r="E19" s="22">
-        <v>3</v>
-      </c>
-      <c r="F19" s="23">
-        <v>44327</v>
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="11">
+        <v>13</v>
+      </c>
+      <c r="E19" s="11">
+        <v>5</v>
+      </c>
+      <c r="F19" s="13">
+        <v>44328</v>
       </c>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="22">
-        <v>13</v>
-      </c>
-      <c r="E20" s="22">
-        <v>4</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="11">
+        <v>5</v>
+      </c>
+      <c r="E20" s="11">
+        <v>8</v>
+      </c>
+      <c r="F20" s="13">
+        <v>44329</v>
       </c>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="11">
-        <v>13</v>
-      </c>
-      <c r="E21" s="11">
-        <v>5</v>
-      </c>
-      <c r="F21" s="14">
-        <v>44328</v>
-      </c>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="11">
-        <v>8</v>
-      </c>
-      <c r="E22" s="11">
-        <v>6</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="11"/>
+      <c r="B21" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="17">
+        <v>44330</v>
+      </c>
+      <c r="G21" s="16">
+        <f>SUM(D16:D20)</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="11">
-        <v>13</v>
-      </c>
-      <c r="E23" s="11">
-        <v>7</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="11"/>
+      <c r="B23" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="11">
-        <v>5</v>
-      </c>
-      <c r="E24" s="11">
-        <v>8</v>
-      </c>
-      <c r="F24" s="14">
-        <v>44329</v>
-      </c>
-      <c r="G24" s="11"/>
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="21">
+        <v>21</v>
+      </c>
+      <c r="E25" s="21">
+        <v>1</v>
+      </c>
+      <c r="F25" s="22">
+        <v>44270</v>
+      </c>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="21">
+        <v>13</v>
+      </c>
+      <c r="E26" s="21">
+        <v>2</v>
+      </c>
+      <c r="F26" s="22">
+        <v>44271</v>
+      </c>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="A27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="21">
+        <v>21</v>
+      </c>
+      <c r="E27" s="21">
+        <v>3</v>
+      </c>
+      <c r="F27" s="22">
+        <v>44271</v>
+      </c>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="18">
-        <v>44330</v>
-      </c>
-      <c r="G25" s="17">
-        <f>SUM(D17:D24)</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="B27" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C28" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="11">
+        <v>8</v>
+      </c>
+      <c r="E28" s="11">
+        <v>7</v>
+      </c>
+      <c r="F28" s="13">
+        <v>44333</v>
+      </c>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="11">
         <v>5</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="22">
-        <v>21</v>
-      </c>
-      <c r="E29" s="22">
-        <v>1</v>
-      </c>
-      <c r="F29" s="23">
-        <v>44270</v>
+      <c r="E29" s="11">
+        <v>8</v>
+      </c>
+      <c r="F29" s="13">
+        <v>44333</v>
       </c>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="22">
-        <v>13</v>
-      </c>
-      <c r="E30" s="22">
-        <v>2</v>
-      </c>
-      <c r="F30" s="23">
-        <v>44271</v>
-      </c>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A31" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="22">
-        <v>21</v>
-      </c>
-      <c r="E31" s="22">
-        <v>3</v>
-      </c>
-      <c r="F31" s="23">
-        <v>44271</v>
-      </c>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="11">
-        <v>8</v>
-      </c>
-      <c r="E32" s="11">
-        <v>4</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="11">
-        <v>13</v>
-      </c>
-      <c r="E33" s="11">
-        <v>5</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A34" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="11">
-        <v>21</v>
-      </c>
-      <c r="E34" s="11">
-        <v>6</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="11">
-        <v>8</v>
-      </c>
-      <c r="E35" s="11">
-        <v>7</v>
-      </c>
-      <c r="F35" s="14">
-        <v>44333</v>
-      </c>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="11">
-        <v>5</v>
-      </c>
-      <c r="E36" s="11">
-        <v>8</v>
-      </c>
-      <c r="F36" s="14">
-        <v>44333</v>
-      </c>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A37" s="7" t="s">
+      <c r="B30" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="17" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F30" s="17">
         <v>44336</v>
       </c>
-      <c r="G37" s="17">
-        <f>SUM(D29:D36)</f>
-        <v>110</v>
+      <c r="G30" s="16">
+        <f>SUM(D25:D29)</f>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>